<commit_message>
Changed the protocol after test run with participant 0 (so this entry won't count) to make the test harder for the participants. I heavn't yet updated the procedure in the writeup
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="2020" yWindow="800" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -33,18 +33,12 @@
     <t>RS-Guess_2</t>
   </si>
   <si>
-    <t>RS-Guess_3</t>
-  </si>
-  <si>
     <t>RS-Sim_1</t>
   </si>
   <si>
     <t>RS-Sim_2</t>
   </si>
   <si>
-    <t>RS-Sim_3</t>
-  </si>
-  <si>
     <t>MPM-Guess_1</t>
   </si>
   <si>
@@ -57,12 +51,6 @@
     <t>MPM-Sim_2</t>
   </si>
   <si>
-    <t>MPM-Guess_3</t>
-  </si>
-  <si>
-    <t>MPM-Sim_3</t>
-  </si>
-  <si>
     <t>RS-Sim_AVG</t>
   </si>
   <si>
@@ -87,12 +75,6 @@
     <t>MX-Sim_2</t>
   </si>
   <si>
-    <t>MX-Guess_3</t>
-  </si>
-  <si>
-    <t>MX-Sim_3</t>
-  </si>
-  <si>
     <t>MX-Sim_AVG</t>
   </si>
   <si>
@@ -100,13 +82,94 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>MPM, MX, RS</t>
+  </si>
+  <si>
+    <t>alotbsol85</t>
+  </si>
+  <si>
+    <t>evildolphinbitesuglyshoe</t>
+  </si>
+  <si>
+    <t>JUs9l^@6t$</t>
+  </si>
+  <si>
+    <t>RS, MX, MPM</t>
+  </si>
+  <si>
+    <t>f,K~ym:}7j</t>
+  </si>
+  <si>
+    <t>MX RS MPM</t>
+  </si>
+  <si>
+    <t>dulldollarshaveshortscience</t>
+  </si>
+  <si>
+    <t>f.K0~n:)7j</t>
+  </si>
+  <si>
+    <t>nastyknightschangepoliteanteater</t>
+  </si>
+  <si>
+    <t>f,K~ym:]7j</t>
+  </si>
+  <si>
+    <t>nastyknightschangetastyanteater</t>
+  </si>
+  <si>
+    <t>\fRRWMM&gt;2,</t>
+  </si>
+  <si>
+    <t>\frrwmm&gt;2,</t>
+  </si>
+  <si>
+    <t>hbty1205</t>
+  </si>
+  <si>
+    <t>tmwt1988</t>
+  </si>
+  <si>
+    <t>MPM MX RS</t>
+  </si>
+  <si>
+    <t>mait10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intelligentballoonsharessillyviolin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">englishrulerunloudwitness </t>
+  </si>
+  <si>
+    <t>Mhm@ujAPOZ</t>
+  </si>
+  <si>
+    <t>Mhm@mjuAPOZ</t>
+  </si>
+  <si>
+    <t>T\YJKwj3Ab</t>
+  </si>
+  <si>
+    <t>Mhm@mujAPOZ</t>
+  </si>
+  <si>
+    <t>V\WYZh13ab</t>
+  </si>
+  <si>
+    <t>mciagb5722</t>
+  </si>
+  <si>
+    <t>T\YZw7j3ab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,6 +201,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -156,7 +226,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -170,26 +240,279 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="139">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -519,31 +842,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H18" sqref="H17:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1">
+    <row r="1" spans="1:21" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -552,25 +881,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
@@ -579,19 +908,19 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>17</v>
@@ -602,23 +931,328 @@
       <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <f>(0.43 + 0.5) / 2</f>
+        <v>0.46499999999999997</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3">
+        <f>(0.9 + 0.82)/2</f>
+        <v>0.86</v>
+      </c>
+      <c r="H3">
+        <f>(E3+G3)/2</f>
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3">
+        <f>(0.42 + 0.75)/2</f>
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="R3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <f>(Q3+S3)/2</f>
+        <v>0.79249999999999998</v>
+      </c>
+      <c r="U3" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4">
+        <f>(0.45+0.5)/2</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f>(E4+G4)/2</f>
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <f>(0.25 + 0.3)/2</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5">
+        <f>(0.6+0.54)/2</f>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="H5">
+        <f>(E5+G5)/2</f>
+        <v>0.42250000000000004</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6">
+        <f>(0.95 + 0.41)/2</f>
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6">
+        <f>(0.95 + 0.45)/2</f>
+        <v>0.7</v>
+      </c>
+      <c r="H6">
+        <f>(E6+G6)/2</f>
+        <v>0.69</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>39</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated acronym in determineOrder and 2 more trials
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="800" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1380" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -163,13 +163,52 @@
   </si>
   <si>
     <t>T\YZw7j3ab</t>
+  </si>
+  <si>
+    <t>RS MPM MX</t>
+  </si>
+  <si>
+    <t>"?za\HNy\n</t>
+  </si>
+  <si>
+    <t>/H/</t>
+  </si>
+  <si>
+    <t>/HNy/</t>
+  </si>
+  <si>
+    <t>sapf11</t>
+  </si>
+  <si>
+    <t>casualpiebecomesonlyprofit</t>
+  </si>
+  <si>
+    <t>plannedaardvarkdrinksbloodyriverbed</t>
+  </si>
+  <si>
+    <t>otherpiebecomesonlyprofit</t>
+  </si>
+  <si>
+    <t>MX MPM RS</t>
+  </si>
+  <si>
+    <t>tirwh31</t>
+  </si>
+  <si>
+    <t>m!WA,SJBPZ</t>
+  </si>
+  <si>
+    <t>*,SJBP</t>
+  </si>
+  <si>
+    <t>!WA,SJBPZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,6 +247,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -226,7 +270,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="139">
+  <cellStyleXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -366,15 +410,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="139">
+  <cellStyles count="151">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -444,6 +501,12 @@
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -513,6 +576,12 @@
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -842,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H18" sqref="H17:H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -860,8 +929,7 @@
     <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -1253,6 +1321,97 @@
       </c>
       <c r="U6" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P7" t="s">
+        <v>55</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="U7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="U8" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filled in calculations for last two trials
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -270,8 +270,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="151">
+  <cellStyleXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -431,7 +493,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="151">
+  <cellStyles count="213">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -507,6 +569,37 @@
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -582,6 +675,37 @@
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -913,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -930,7 +1054,7 @@
     <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1333,9 +1457,21 @@
       <c r="D7" t="s">
         <v>50</v>
       </c>
+      <c r="E7">
+        <f>0.1/2</f>
+        <v>0.05</v>
+      </c>
       <c r="F7" t="s">
         <v>51</v>
       </c>
+      <c r="G7">
+        <f>0.3/2</f>
+        <v>0.15</v>
+      </c>
+      <c r="H7">
+        <f>(E7+G7)/2</f>
+        <v>0.1</v>
+      </c>
       <c r="I7" t="s">
         <v>52</v>
       </c>
@@ -1360,11 +1496,19 @@
       <c r="P7" t="s">
         <v>55</v>
       </c>
+      <c r="Q7">
+        <f>(0.38 + 0.75)/2</f>
+        <v>0.56499999999999995</v>
+      </c>
       <c r="R7" s="3" t="s">
         <v>53</v>
       </c>
       <c r="S7">
         <v>1</v>
+      </c>
+      <c r="T7">
+        <f>(Q7+S7)/2</f>
+        <v>0.78249999999999997</v>
       </c>
       <c r="U7" t="s">
         <v>48</v>
@@ -1380,9 +1524,21 @@
       <c r="D8" t="s">
         <v>59</v>
       </c>
+      <c r="E8">
+        <f>0.45/2</f>
+        <v>0.22500000000000001</v>
+      </c>
       <c r="F8" t="s">
         <v>60</v>
       </c>
+      <c r="G8">
+        <f>(0.9+0.45)/2</f>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="H8">
+        <f>(E8+G8)/2</f>
+        <v>0.45</v>
+      </c>
       <c r="I8" t="s">
         <v>57</v>
       </c>
@@ -1408,6 +1564,15 @@
         <v>54</v>
       </c>
       <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>54</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
         <v>1</v>
       </c>
       <c r="U8" t="s">

</xml_diff>

<commit_message>
Added entropy calculations to results spreadsheet
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2520" yWindow="860" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>);\U)nd&gt;N^</t>
+  </si>
+  <si>
+    <t>RS-Entropy</t>
+  </si>
+  <si>
+    <t>MX-Entropy</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>MPM-Entropy</t>
   </si>
 </sst>
 </file>
@@ -1110,32 +1122,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="38.1640625" customWidth="1"/>
+    <col min="18" max="18" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1">
+    <row r="1" spans="1:23" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1143,90 +1158,101 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:23">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <f>94^10</f>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>21</v>
+      <c r="H2">
+        <v>1</v>
       </c>
       <c r="I2" t="s">
         <v>21</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <f>(26^8)*(10^2)</f>
+        <v>20882706457600</v>
       </c>
       <c r="K2" t="s">
         <v>21</v>
@@ -1234,64 +1260,76 @@
       <c r="L2">
         <v>1</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
         <v>22</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2">
+        <f>26^LEN(P2)</f>
+        <v>9.1066857695372161E+33</v>
+      </c>
+      <c r="R2" t="s">
         <v>22</v>
       </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
         <v>22</v>
       </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <f t="shared" ref="C3:C9" si="0">94^10</f>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <f>(0.43 + 0.5) / 2</f>
         <v>0.46499999999999997</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>30</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <f>(0.9 + 0.82)/2</f>
         <v>0.86</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G8" si="0">(D3+F3)/2</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H8" si="1">(E3+G3)/2</f>
         <v>0.66249999999999998</v>
-      </c>
-      <c r="H3" t="s">
-        <v>35</v>
       </c>
       <c r="I3" t="s">
         <v>35</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <f>(26^4)*(10^4)</f>
+        <v>4569760000</v>
       </c>
       <c r="K3" t="s">
         <v>35</v>
@@ -1299,65 +1337,77 @@
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
         <v>29</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q9" si="2">26^LEN(P3)</f>
+        <v>1.9017224572684885E+45</v>
+      </c>
+      <c r="R3" t="s">
         <v>31</v>
       </c>
-      <c r="P3">
+      <c r="S3">
         <f>(0.42 + 0.75)/2</f>
         <v>0.58499999999999996</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>29</v>
       </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <f>(P3+R3)/2</f>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <f>(S3+U3)/2</f>
         <v>0.79249999999999998</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:23">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f>(0.45+0.5)/2</f>
         <v>0.47499999999999998</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>32</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
         <v>0.73750000000000004</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
       </c>
       <c r="I4" t="s">
         <v>34</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <f>(26^4)*(10^4)</f>
+        <v>4569760000</v>
       </c>
       <c r="K4" t="s">
         <v>34</v>
@@ -1365,64 +1415,76 @@
       <c r="L4">
         <v>1</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
         <v>27</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4">
+        <f t="shared" si="2"/>
+        <v>1.6005910908538611E+38</v>
+      </c>
+      <c r="R4" t="s">
         <v>27</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
         <v>27</v>
       </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:23">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D5" t="s">
         <v>44</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f>(0.25 + 0.3)/2</f>
         <v>0.27500000000000002</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>46</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f>(0.6+0.54)/2</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
+      <c r="H5">
+        <f t="shared" si="1"/>
         <v>0.42250000000000004</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
       </c>
       <c r="I5" t="s">
         <v>37</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <f>(26^4)*(10^2)</f>
+        <v>45697600</v>
       </c>
       <c r="K5" t="s">
         <v>37</v>
@@ -1430,64 +1492,76 @@
       <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="M5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
         <v>39</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5">
+        <f t="shared" si="2"/>
+        <v>6.1561195802071578E+36</v>
+      </c>
+      <c r="R5" t="s">
         <v>39</v>
       </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
         <v>39</v>
       </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:23">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f>(0.95 + 0.41)/2</f>
         <v>0.67999999999999994</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>43</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f>(0.95 + 0.45)/2</f>
         <v>0.7</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
+      <c r="H6">
+        <f t="shared" si="1"/>
         <v>0.69</v>
-      </c>
-      <c r="H6" t="s">
-        <v>45</v>
       </c>
       <c r="I6" t="s">
         <v>45</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <f>(26^6)*(10^4)</f>
+        <v>3089157760000</v>
       </c>
       <c r="K6" t="s">
         <v>45</v>
@@ -1495,64 +1569,76 @@
       <c r="L6">
         <v>1</v>
       </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="M6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
         <v>38</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6">
+        <f t="shared" si="2"/>
+        <v>8.6904152163272471E+50</v>
+      </c>
+      <c r="R6" t="s">
         <v>38</v>
       </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
         <v>38</v>
       </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:23">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D7" t="s">
         <v>49</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f>0.1/2</f>
         <v>0.05</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>50</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <f>0.3/2</f>
         <v>0.15</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
+      <c r="H7">
+        <f t="shared" si="1"/>
         <v>0.1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>51</v>
       </c>
       <c r="I7" t="s">
         <v>51</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <f>(26^4)*(10^2)</f>
+        <v>45697600</v>
       </c>
       <c r="K7" t="s">
         <v>51</v>
@@ -1560,66 +1646,78 @@
       <c r="L7">
         <v>1</v>
       </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" s="3" t="s">
+      <c r="M7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7">
+        <f t="shared" si="2"/>
+        <v>6.1561195802071578E+36</v>
+      </c>
+      <c r="R7" t="s">
         <v>54</v>
       </c>
-      <c r="P7">
+      <c r="S7">
         <f>(0.38 + 0.75)/2</f>
         <v>0.56499999999999995</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="T7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <f>(P7+R7)/2</f>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <f>(S7+U7)/2</f>
         <v>0.78249999999999997</v>
       </c>
-      <c r="T7" t="s">
+      <c r="W7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:23">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>57</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D8" t="s">
         <v>58</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f>0.45/2</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>59</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f>(0.9+0.45)/2</f>
         <v>0.67500000000000004</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
+      <c r="H8">
+        <f t="shared" si="1"/>
         <v>0.45</v>
-      </c>
-      <c r="H8" t="s">
-        <v>56</v>
       </c>
       <c r="I8" t="s">
         <v>56</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <f>(26^6)*(10^2)</f>
+        <v>30891577600</v>
       </c>
       <c r="K8" t="s">
         <v>56</v>
@@ -1627,64 +1725,76 @@
       <c r="L8">
         <v>1</v>
       </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="M8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
         <v>53</v>
       </c>
-      <c r="O8" t="s">
+      <c r="Q8">
+        <f t="shared" si="2"/>
+        <v>3.3424673908950952E+49</v>
+      </c>
+      <c r="R8" t="s">
         <v>53</v>
       </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
         <v>53</v>
       </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:23">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D9" t="s">
         <v>64</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f>(0.6 + 0.35)/2</f>
         <v>0.47499999999999998</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>65</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f>(0.7+0.8)/2</f>
         <v>0.75</v>
       </c>
-      <c r="G9">
-        <f>(D9+F9)/2</f>
+      <c r="H9">
+        <f>(E9+G9)/2</f>
         <v>0.61250000000000004</v>
-      </c>
-      <c r="H9" t="s">
-        <v>60</v>
       </c>
       <c r="I9" t="s">
         <v>60</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <f>(26^5)*(10^4)</f>
+        <v>118813760000</v>
       </c>
       <c r="K9" t="s">
         <v>60</v>
@@ -1692,31 +1802,58 @@
       <c r="L9">
         <v>1</v>
       </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9" s="2" t="s">
+      <c r="M9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9">
+        <f t="shared" si="2"/>
+        <v>3.9713111838963607E+56</v>
+      </c>
+      <c r="R9" t="s">
         <v>62</v>
       </c>
-      <c r="P9">
+      <c r="S9">
         <f>(0.5 + 0.09)/2</f>
         <v>0.29499999999999998</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="T9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9">
-        <f>(P9+R9)/2</f>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <f>(S9+U9)/2</f>
         <v>0.64749999999999996</v>
       </c>
-      <c r="T9" t="s">
+      <c r="W9" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10">
+        <f>AVERAGE(C2:C9)</f>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="J10">
+        <f>AVERAGE(J2:J9)</f>
+        <v>3016350058800</v>
+      </c>
+      <c r="Q10">
+        <f>AVERAGE(Q2:Q9)</f>
+        <v>4.9641502607216668E+55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated procedure. And added stdev and averages to similarity percentages
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="860" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1460" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -229,6 +229,15 @@
   </si>
   <si>
     <t>MPM-Entropy</t>
+  </si>
+  <si>
+    <t>RS-Sim_STD</t>
+  </si>
+  <si>
+    <t>MPM-Sim_STD</t>
+  </si>
+  <si>
+    <t>MX-Sim-STD</t>
   </si>
 </sst>
 </file>
@@ -297,8 +306,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="243">
+  <cellStyleXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -550,7 +573,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="243">
+  <cellStyles count="257">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -672,6 +695,13 @@
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -793,6 +823,13 @@
     <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1122,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1136,21 +1173,23 @@
     <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="38.1640625" customWidth="1"/>
-    <col min="18" max="18" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" customWidth="1"/>
+    <col min="18" max="18" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.1640625" customWidth="1"/>
+    <col min="20" max="20" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.5" customWidth="1"/>
+    <col min="26" max="26" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1">
+    <row r="1" spans="1:26" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1176,52 +1215,61 @@
         <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:26">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1247,40 +1295,42 @@
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2">
+        <f>STDEV(G2:H2)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <f>(26^8)*(10^2)</f>
         <v>20882706457600</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
         <v>21</v>
       </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
-        <v>22</v>
+      <c r="P2">
+        <v>1</v>
       </c>
       <c r="Q2">
-        <f>26^LEN(P2)</f>
-        <v>9.1066857695372161E+33</v>
+        <f>STDEV(O2:P2)</f>
+        <v>0</v>
       </c>
       <c r="R2" t="s">
         <v>22</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <f>26^LEN(R2)</f>
+        <v>9.1066857695372161E+33</v>
       </c>
       <c r="T2" t="s">
         <v>22</v>
@@ -1288,14 +1338,24 @@
       <c r="U2">
         <v>1</v>
       </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="V2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <f>STDEV(W2:X2)</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:26">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1324,57 +1384,69 @@
         <f t="shared" ref="H3:H8" si="1">(E3+G3)/2</f>
         <v>0.66249999999999998</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3">
+        <f t="shared" ref="I3:I9" si="2">STDEV(G3:H3)</f>
+        <v>0.13965358928434296</v>
+      </c>
+      <c r="J3" t="s">
         <v>35</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <f>(26^4)*(10^4)</f>
         <v>4569760000</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>35</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
         <v>35</v>
       </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q9" si="3">STDEV(O3:P3)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" t="s">
         <v>29</v>
       </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q9" si="2">26^LEN(P3)</f>
+      <c r="S3">
+        <f t="shared" ref="S3:S9" si="4">26^LEN(R3)</f>
         <v>1.9017224572684885E+45</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>31</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <f>(0.42 + 0.75)/2</f>
         <v>0.58499999999999996</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>29</v>
       </c>
-      <c r="U3">
-        <v>1</v>
-      </c>
-      <c r="V3">
-        <f>(S3+U3)/2</f>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <f>(U3+W3)/2</f>
         <v>0.79249999999999998</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y9" si="5">STDEV(W3:X3)</f>
+        <v>0.14672465709620902</v>
+      </c>
+      <c r="Z3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:26">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1402,40 +1474,42 @@
         <f t="shared" si="1"/>
         <v>0.73750000000000004</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0.18561553006146866</v>
+      </c>
+      <c r="J4" t="s">
         <v>34</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f>(26^4)*(10^4)</f>
         <v>4569760000</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>34</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
         <v>34</v>
       </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
       <c r="O4">
         <v>1</v>
       </c>
-      <c r="P4" t="s">
-        <v>27</v>
+      <c r="P4">
+        <v>1</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="2"/>
-        <v>1.6005910908538611E+38</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="R4" t="s">
         <v>27</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>1.6005910908538611E+38</v>
       </c>
       <c r="T4" t="s">
         <v>27</v>
@@ -1443,14 +1517,24 @@
       <c r="U4">
         <v>1</v>
       </c>
-      <c r="V4">
-        <v>1</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="V4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:26">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1479,40 +1563,42 @@
         <f t="shared" si="1"/>
         <v>0.42250000000000004</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>0.10429825022501531</v>
+      </c>
+      <c r="J5" t="s">
         <v>37</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f>(26^4)*(10^2)</f>
         <v>45697600</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>37</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
         <v>37</v>
       </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="P5" t="s">
-        <v>39</v>
+      <c r="P5">
+        <v>1</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="2"/>
-        <v>6.1561195802071578E+36</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="R5" t="s">
         <v>39</v>
       </c>
       <c r="S5">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>6.1561195802071578E+36</v>
       </c>
       <c r="T5" t="s">
         <v>39</v>
@@ -1520,14 +1606,24 @@
       <c r="U5">
         <v>1</v>
       </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="V5" t="s">
+        <v>39</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:26">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1556,40 +1652,42 @@
         <f t="shared" si="1"/>
         <v>0.69</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>7.0710678118654814E-3</v>
+      </c>
+      <c r="J6" t="s">
         <v>45</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f>(26^6)*(10^4)</f>
         <v>3089157760000</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>45</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
         <v>45</v>
       </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
       <c r="O6">
         <v>1</v>
       </c>
-      <c r="P6" t="s">
-        <v>38</v>
+      <c r="P6">
+        <v>1</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="2"/>
-        <v>8.6904152163272471E+50</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="R6" t="s">
         <v>38</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>8.6904152163272471E+50</v>
       </c>
       <c r="T6" t="s">
         <v>38</v>
@@ -1597,14 +1695,24 @@
       <c r="U6">
         <v>1</v>
       </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="V6" t="s">
+        <v>38</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:26">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1633,57 +1741,69 @@
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>3.535533905932739E-2</v>
+      </c>
+      <c r="J7" t="s">
         <v>51</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f>(26^4)*(10^2)</f>
         <v>45697600</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>51</v>
       </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
         <v>51</v>
       </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
       <c r="O7">
         <v>1</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q7">
-        <f t="shared" si="2"/>
+      <c r="S7">
+        <f t="shared" si="4"/>
         <v>6.1561195802071578E+36</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>54</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <f>(0.38 + 0.75)/2</f>
         <v>0.56499999999999995</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="V7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="U7">
-        <v>1</v>
-      </c>
-      <c r="V7">
-        <f>(S7+U7)/2</f>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <f>(U7+W7)/2</f>
         <v>0.78249999999999997</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Y7">
+        <f t="shared" si="5"/>
+        <v>0.15379572490807425</v>
+      </c>
+      <c r="Z7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:26">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1712,40 +1832,42 @@
         <f t="shared" si="1"/>
         <v>0.45</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>0.15909902576697341</v>
+      </c>
+      <c r="J8" t="s">
         <v>56</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f>(26^6)*(10^2)</f>
         <v>30891577600</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>56</v>
       </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
         <v>56</v>
       </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
       <c r="O8">
         <v>1</v>
       </c>
-      <c r="P8" t="s">
-        <v>53</v>
+      <c r="P8">
+        <v>1</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="2"/>
-        <v>3.3424673908950952E+49</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="R8" t="s">
         <v>53</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>3.3424673908950952E+49</v>
       </c>
       <c r="T8" t="s">
         <v>53</v>
@@ -1753,14 +1875,24 @@
       <c r="U8">
         <v>1</v>
       </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
-      <c r="W8" t="s">
+      <c r="V8" t="s">
+        <v>53</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:26">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1789,57 +1921,69 @@
         <f>(E9+G9)/2</f>
         <v>0.61250000000000004</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>9.7227182413150606E-2</v>
+      </c>
+      <c r="J9" t="s">
         <v>60</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f>(26^5)*(10^4)</f>
         <v>118813760000</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>60</v>
       </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
         <v>60</v>
       </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
       <c r="O9">
         <v>1</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Q9">
-        <f t="shared" si="2"/>
+      <c r="S9">
+        <f t="shared" si="4"/>
         <v>3.9713111838963607E+56</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>62</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <f>(0.5 + 0.09)/2</f>
         <v>0.29499999999999998</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="V9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="U9">
-        <v>1</v>
-      </c>
-      <c r="V9">
-        <f>(S9+U9)/2</f>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <f>(U9+W9)/2</f>
         <v>0.64749999999999996</v>
       </c>
-      <c r="W9" t="s">
+      <c r="Y9">
+        <f t="shared" si="5"/>
+        <v>0.24925514036825774</v>
+      </c>
+      <c r="Z9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -1847,13 +1991,61 @@
         <f>AVERAGE(C2:C9)</f>
         <v>5.3861511409489969E+19</v>
       </c>
-      <c r="J10">
-        <f>AVERAGE(J2:J9)</f>
+      <c r="E10">
+        <f>AVERAGE(E2:E9)</f>
+        <v>0.45562499999999995</v>
+      </c>
+      <c r="G10">
+        <f>AVERAGE(G2:G9)</f>
+        <v>0.71312500000000001</v>
+      </c>
+      <c r="H10">
+        <f>AVERAGE(H2:H9)</f>
+        <v>0.58437499999999998</v>
+      </c>
+      <c r="I10">
+        <f>AVERAGE(I2:I9)</f>
+        <v>9.1039998077767983E-2</v>
+      </c>
+      <c r="K10">
+        <f>AVERAGE(K2:K9)</f>
         <v>3016350058800</v>
+      </c>
+      <c r="M10">
+        <f>AVERAGE(M2:M9)</f>
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <f>AVERAGE(O2:O9)</f>
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f>AVERAGE(P2:P9)</f>
+        <v>1</v>
       </c>
       <c r="Q10">
         <f>AVERAGE(Q2:Q9)</f>
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f>AVERAGE(S2:S9)</f>
         <v>4.9641502607216668E+55</v>
+      </c>
+      <c r="U10">
+        <f>AVERAGE(U2:U9)</f>
+        <v>0.80562500000000004</v>
+      </c>
+      <c r="W10">
+        <f>AVERAGE(W2:W9)</f>
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <f>AVERAGE(X2:X9)</f>
+        <v>0.90281250000000002</v>
+      </c>
+      <c r="Y10">
+        <f>AVERAGE(Y2:Y9)</f>
+        <v>6.8721940296567627E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed STDEV calculations (it was avg. and second trial, now it's 1st trial and second trial
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -1162,7 +1162,7 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1296,7 +1296,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <f>STDEV(G2:H2)</f>
+        <f>STDEV(E2,G2)</f>
         <v>0</v>
       </c>
       <c r="J2" t="s">
@@ -1322,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="Q2">
-        <f>STDEV(O2:P2)</f>
+        <f>STDEV(M2,O2)</f>
         <v>0</v>
       </c>
       <c r="R2" t="s">
@@ -1348,7 +1348,7 @@
         <v>1</v>
       </c>
       <c r="Y2">
-        <f>STDEV(W2:X2)</f>
+        <f>STDEV(U2, W2)</f>
         <v>0</v>
       </c>
       <c r="Z2" t="s">
@@ -1385,8 +1385,8 @@
         <v>0.66249999999999998</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I9" si="2">STDEV(G3:H3)</f>
-        <v>0.13965358928434296</v>
+        <f t="shared" ref="I3:I9" si="2">STDEV(E3,G3)</f>
+        <v>0.27930717856868614</v>
       </c>
       <c r="J3" t="s">
         <v>35</v>
@@ -1411,7 +1411,7 @@
         <v>1</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q9" si="3">STDEV(O3:P3)</f>
+        <f t="shared" ref="Q3:Q9" si="3">STDEV(M3,O3)</f>
         <v>0</v>
       </c>
       <c r="R3" t="s">
@@ -1439,8 +1439,8 @@
         <v>0.79249999999999998</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y9" si="5">STDEV(W3:X3)</f>
-        <v>0.14672465709620902</v>
+        <f t="shared" ref="Y3:Y9" si="5">STDEV(U3, W3)</f>
+        <v>0.29344931419241727</v>
       </c>
       <c r="Z3" t="s">
         <v>24</v>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="I4">
         <f t="shared" si="2"/>
-        <v>0.18561553006146866</v>
+        <v>0.37123106012293733</v>
       </c>
       <c r="J4" t="s">
         <v>34</v>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>0.10429825022501531</v>
+        <v>0.20859650045003153</v>
       </c>
       <c r="J5" t="s">
         <v>37</v>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
-        <v>7.0710678118654814E-3</v>
+        <v>1.4142135623730963E-2</v>
       </c>
       <c r="J6" t="s">
         <v>45</v>
@@ -1743,7 +1743,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>3.535533905932739E-2</v>
+        <v>7.0710678118654738E-2</v>
       </c>
       <c r="J7" t="s">
         <v>51</v>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="Y7">
         <f t="shared" si="5"/>
-        <v>0.15379572490807425</v>
+        <v>0.30759144981614817</v>
       </c>
       <c r="Z7" t="s">
         <v>47</v>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="I8">
         <f t="shared" si="2"/>
-        <v>0.15909902576697341</v>
+        <v>0.31819805153394648</v>
       </c>
       <c r="J8" t="s">
         <v>56</v>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>9.7227182413150606E-2</v>
+        <v>0.19445436482630007</v>
       </c>
       <c r="J9" t="s">
         <v>60</v>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="Y9">
         <f t="shared" si="5"/>
-        <v>0.24925514036825774</v>
+        <v>0.49851028073651604</v>
       </c>
       <c r="Z9" t="s">
         <v>36</v>
@@ -2005,7 +2005,7 @@
       </c>
       <c r="I10">
         <f>AVERAGE(I2:I9)</f>
-        <v>9.1039998077767983E-2</v>
+        <v>0.18207999615553588</v>
       </c>
       <c r="K10">
         <f>AVERAGE(K2:K9)</f>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="Y10">
         <f>AVERAGE(Y2:Y9)</f>
-        <v>6.8721940296567627E-2</v>
+        <v>0.13744388059313517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added average percent change between trials, implies people learn MX faster than RS. Only included trials in which they didn't get it perfectly on both trials
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -238,6 +238,18 @@
   </si>
   <si>
     <t>MX-Sim-STD</t>
+  </si>
+  <si>
+    <t>RS-Imprv</t>
+  </si>
+  <si>
+    <t>MPM-Imprv</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>MX-Imprv</t>
   </si>
 </sst>
 </file>
@@ -306,8 +318,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="257">
+  <cellStyleXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -573,7 +603,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="257">
+  <cellStyles count="275">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -702,6 +732,15 @@
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -830,6 +869,15 @@
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1159,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1172,24 +1220,25 @@
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" customWidth="1"/>
-    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.1640625" customWidth="1"/>
-    <col min="18" max="18" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="38.1640625" customWidth="1"/>
-    <col min="20" max="20" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5" customWidth="1"/>
-    <col min="26" max="26" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" customWidth="1"/>
+    <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1640625" customWidth="1"/>
+    <col min="20" max="20" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="38.1640625" customWidth="1"/>
+    <col min="22" max="22" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.5" customWidth="1"/>
+    <col min="29" max="29" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1">
+    <row r="1" spans="1:29" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1212,64 +1261,73 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:29">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1293,50 +1351,51 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <f>G2-E2</f>
+        <v>0</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <f>STDEV(E2,G2)</f>
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <f>(26^8)*(10^2)</f>
         <v>20882706457600</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>21</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
         <v>21</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
       <c r="P2">
         <v>1</v>
       </c>
-      <c r="Q2">
-        <f>STDEV(M2,O2)</f>
+      <c r="Q2" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <f>STDEV(N2,P2)</f>
         <v>0</v>
-      </c>
-      <c r="R2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2">
-        <f>26^LEN(R2)</f>
-        <v>9.1066857695372161E+33</v>
       </c>
       <c r="T2" t="s">
         <v>22</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <f>26^LEN(T2)</f>
+        <v>9.1066857695372161E+33</v>
       </c>
       <c r="V2" t="s">
         <v>22</v>
@@ -1344,18 +1403,27 @@
       <c r="W2">
         <v>1</v>
       </c>
-      <c r="X2">
-        <v>1</v>
+      <c r="X2" t="s">
+        <v>22</v>
       </c>
       <c r="Y2">
-        <f>STDEV(U2, W2)</f>
+        <v>1</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <f>STDEV(W2, Y2)</f>
         <v>0</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AC2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:29">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1381,72 +1449,83 @@
         <v>0.86</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H8" si="1">(E3+G3)/2</f>
+        <f t="shared" ref="H3:H9" si="1">G3-E3</f>
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="I3">
+        <f>(E3+G3)/2</f>
         <v>0.66249999999999998</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I9" si="2">STDEV(E3,G3)</f>
+      <c r="J3">
+        <f>STDEV(E3,G3)</f>
         <v>0.27930717856868614</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>35</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <f>(26^4)*(10^4)</f>
         <v>4569760000</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>35</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
         <v>35</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
       <c r="P3">
         <v>1</v>
       </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q9" si="3">STDEV(M3,O3)</f>
+      <c r="Q3" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S9" si="2">STDEV(N3,P3)</f>
         <v>0</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>29</v>
       </c>
-      <c r="S3">
-        <f t="shared" ref="S3:S9" si="4">26^LEN(R3)</f>
+      <c r="U3">
+        <f t="shared" ref="U3:U9" si="3">26^LEN(T3)</f>
         <v>1.9017224572684885E+45</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>31</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <f>(0.42 + 0.75)/2</f>
         <v>0.58499999999999996</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
         <v>29</v>
       </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
-      <c r="X3">
-        <f>(U3+W3)/2</f>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <f>Y3-W3</f>
+        <v>0.41500000000000004</v>
+      </c>
+      <c r="AA3">
+        <f>(W3+Y3)/2</f>
         <v>0.79249999999999998</v>
       </c>
-      <c r="Y3">
-        <f t="shared" ref="Y3:Y9" si="5">STDEV(U3, W3)</f>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB9" si="4">STDEV(W3, Y3)</f>
         <v>0.29344931419241727</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AC3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:29">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1472,50 +1551,51 @@
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="I4">
+        <f>(E4+G4)/2</f>
         <v>0.73750000000000004</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="2"/>
+      <c r="J4">
+        <f>STDEV(E4,G4)</f>
         <v>0.37123106012293733</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>34</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f>(26^4)*(10^4)</f>
         <v>4569760000</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>34</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
         <v>34</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
       <c r="P4">
         <v>1</v>
       </c>
-      <c r="Q4">
-        <f t="shared" si="3"/>
+      <c r="Q4" t="s">
+        <v>75</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4">
-        <f t="shared" si="4"/>
-        <v>1.6005910908538611E+38</v>
       </c>
       <c r="T4" t="s">
         <v>27</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>1.6005910908538611E+38</v>
       </c>
       <c r="V4" t="s">
         <v>27</v>
@@ -1523,18 +1603,27 @@
       <c r="W4">
         <v>1</v>
       </c>
-      <c r="X4">
-        <v>1</v>
+      <c r="X4" t="s">
+        <v>27</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AC4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:29">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1561,50 +1650,51 @@
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
+        <v>0.29500000000000004</v>
+      </c>
+      <c r="I5">
+        <f>(E5+G5)/2</f>
         <v>0.42250000000000004</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="2"/>
+      <c r="J5">
+        <f>STDEV(E5,G5)</f>
         <v>0.20859650045003153</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>37</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <f>(26^4)*(10^2)</f>
         <v>45697600</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>37</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
         <v>37</v>
       </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
       <c r="P5">
         <v>1</v>
       </c>
-      <c r="Q5">
-        <f t="shared" si="3"/>
+      <c r="Q5" t="s">
+        <v>75</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="R5" t="s">
-        <v>39</v>
-      </c>
-      <c r="S5">
-        <f t="shared" si="4"/>
-        <v>6.1561195802071578E+36</v>
       </c>
       <c r="T5" t="s">
         <v>39</v>
       </c>
       <c r="U5">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>6.1561195802071578E+36</v>
       </c>
       <c r="V5" t="s">
         <v>39</v>
@@ -1612,18 +1702,27 @@
       <c r="W5">
         <v>1</v>
       </c>
-      <c r="X5">
-        <v>1</v>
+      <c r="X5" t="s">
+        <v>39</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AC5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1650,50 +1749,51 @@
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="I6">
+        <f>(E6+G6)/2</f>
         <v>0.69</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="2"/>
+      <c r="J6">
+        <f>STDEV(E6,G6)</f>
         <v>1.4142135623730963E-2</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>45</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <f>(26^6)*(10^4)</f>
         <v>3089157760000</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>45</v>
       </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
         <v>45</v>
       </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
       <c r="P6">
         <v>1</v>
       </c>
-      <c r="Q6">
-        <f t="shared" si="3"/>
+      <c r="Q6" t="s">
+        <v>75</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="R6" t="s">
-        <v>38</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="4"/>
-        <v>8.6904152163272471E+50</v>
       </c>
       <c r="T6" t="s">
         <v>38</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>8.6904152163272471E+50</v>
       </c>
       <c r="V6" t="s">
         <v>38</v>
@@ -1701,18 +1801,27 @@
       <c r="W6">
         <v>1</v>
       </c>
-      <c r="X6">
-        <v>1</v>
+      <c r="X6" t="s">
+        <v>38</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AC6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1739,71 +1848,82 @@
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="I7">
+        <f>(E7+G7)/2</f>
         <v>0.1</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="2"/>
+      <c r="J7">
+        <f>STDEV(E7,G7)</f>
         <v>7.0710678118654738E-2</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>51</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f>(26^4)*(10^2)</f>
         <v>45697600</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>51</v>
       </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
         <v>51</v>
       </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
       <c r="P7">
         <v>1</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" t="s">
+        <v>75</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="U7">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="4"/>
         <v>6.1561195802071578E+36</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>54</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <f>(0.38 + 0.75)/2</f>
         <v>0.56499999999999995</v>
       </c>
-      <c r="V7" s="3" t="s">
+      <c r="X7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W7">
-        <v>1</v>
-      </c>
-      <c r="X7">
-        <f>(U7+W7)/2</f>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <f>Y7-W7</f>
+        <v>0.43500000000000005</v>
+      </c>
+      <c r="AA7">
+        <f>(W7+Y7)/2</f>
         <v>0.78249999999999997</v>
       </c>
-      <c r="Y7">
-        <f t="shared" si="5"/>
+      <c r="AB7">
+        <f t="shared" si="4"/>
         <v>0.30759144981614817</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AC7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1830,50 +1950,51 @@
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
+        <v>0.45000000000000007</v>
+      </c>
+      <c r="I8">
+        <f>(E8+G8)/2</f>
         <v>0.45</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="2"/>
+      <c r="J8">
+        <f>STDEV(E8,G8)</f>
         <v>0.31819805153394648</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>56</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <f>(26^6)*(10^2)</f>
         <v>30891577600</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>56</v>
       </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
         <v>56</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
       <c r="P8">
         <v>1</v>
       </c>
-      <c r="Q8">
-        <f t="shared" si="3"/>
+      <c r="Q8" t="s">
+        <v>75</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
         <v>0</v>
-      </c>
-      <c r="R8" t="s">
-        <v>53</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="4"/>
-        <v>3.3424673908950952E+49</v>
       </c>
       <c r="T8" t="s">
         <v>53</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>3.3424673908950952E+49</v>
       </c>
       <c r="V8" t="s">
         <v>53</v>
@@ -1881,18 +2002,27 @@
       <c r="W8">
         <v>1</v>
       </c>
-      <c r="X8">
-        <v>1</v>
+      <c r="X8" t="s">
+        <v>53</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AC8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1918,72 +2048,83 @@
         <v>0.75</v>
       </c>
       <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="I9">
         <f>(E9+G9)/2</f>
         <v>0.61250000000000004</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="2"/>
+      <c r="J9">
+        <f>STDEV(E9,G9)</f>
         <v>0.19445436482630007</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>60</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <f>(26^5)*(10^4)</f>
         <v>118813760000</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>60</v>
       </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
         <v>60</v>
       </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
       <c r="P9">
         <v>1</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" t="s">
+        <v>75</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="U9">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="4"/>
         <v>3.9713111838963607E+56</v>
       </c>
-      <c r="T9" t="s">
+      <c r="V9" t="s">
         <v>62</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <f>(0.5 + 0.09)/2</f>
         <v>0.29499999999999998</v>
       </c>
-      <c r="V9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="W9">
-        <v>1</v>
-      </c>
-      <c r="X9">
-        <f>(U9+W9)/2</f>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <f>Y9-W9</f>
+        <v>0.70500000000000007</v>
+      </c>
+      <c r="AA9">
+        <f>(W9+Y9)/2</f>
         <v>0.64749999999999996</v>
       </c>
-      <c r="Y9">
-        <f t="shared" si="5"/>
+      <c r="AB9">
+        <f t="shared" si="4"/>
         <v>0.49851028073651604</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AC9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -2001,50 +2142,61 @@
       </c>
       <c r="H10">
         <f>AVERAGE(H2:H9)</f>
-        <v>0.58437499999999998</v>
+        <v>0.25750000000000001</v>
       </c>
       <c r="I10">
         <f>AVERAGE(I2:I9)</f>
+        <v>0.58437499999999998</v>
+      </c>
+      <c r="J10">
+        <f>AVERAGE(J2:J9)</f>
         <v>0.18207999615553588</v>
       </c>
-      <c r="K10">
-        <f>AVERAGE(K2:K9)</f>
+      <c r="L10">
+        <f>AVERAGE(L2:L9)</f>
         <v>3016350058800</v>
       </c>
-      <c r="M10">
-        <f>AVERAGE(M2:M9)</f>
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <f>AVERAGE(O2:O9)</f>
+      <c r="N10">
+        <f>AVERAGE(N2:N9)</f>
         <v>1</v>
       </c>
       <c r="P10">
         <f>AVERAGE(P2:P9)</f>
         <v>1</v>
       </c>
-      <c r="Q10">
-        <f>AVERAGE(Q2:Q9)</f>
-        <v>0</v>
+      <c r="Q10" t="s">
+        <v>75</v>
+      </c>
+      <c r="R10">
+        <f>AVERAGE(R2:R9)</f>
+        <v>1</v>
       </c>
       <c r="S10">
         <f>AVERAGE(S2:S9)</f>
-        <v>4.9641502607216668E+55</v>
+        <v>0</v>
       </c>
       <c r="U10">
         <f>AVERAGE(U2:U9)</f>
-        <v>0.80562500000000004</v>
+        <v>4.9641502607216668E+55</v>
       </c>
       <c r="W10">
         <f>AVERAGE(W2:W9)</f>
-        <v>1</v>
-      </c>
-      <c r="X10">
-        <f>AVERAGE(X2:X9)</f>
-        <v>0.90281250000000002</v>
+        <v>0.80562500000000004</v>
       </c>
       <c r="Y10">
         <f>AVERAGE(Y2:Y9)</f>
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <f>AVERAGE(Z3,Z7,Z9)</f>
+        <v>0.51833333333333342</v>
+      </c>
+      <c r="AA10">
+        <f>AVERAGE(AA2:AA9)</f>
+        <v>0.90281250000000002</v>
+      </c>
+      <c r="AB10">
+        <f>AVERAGE(AB2:AB9)</f>
         <v>0.13744388059313517</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created summary, learning gains, and nhtropy graphs in results
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -4,10 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1460" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Entropy Graph" sheetId="2" r:id="rId2"/>
+    <sheet name="Avg Tests" sheetId="3" r:id="rId3"/>
+    <sheet name="Learning Gains" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -250,6 +253,39 @@
   </si>
   <si>
     <t>MX-Imprv</t>
+  </si>
+  <si>
+    <t>Password Type</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>MPM</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>log_10 Entropy</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password </t>
+  </si>
+  <si>
+    <t>Second Trial</t>
+  </si>
+  <si>
+    <t>First Trial</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Improvement</t>
   </si>
 </sst>
 </file>
@@ -318,8 +354,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="275">
+  <cellStyleXfs count="311">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -603,7 +675,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="275">
+  <cellStyles count="311">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -741,6 +813,24 @@
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -878,11 +968,761 @@
     <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Entropy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Passwords</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Entropy Graph'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>log_10 Entropy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Entropy Graph'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>RS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MPM</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MX</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Entropy Graph'!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>19.73127853599699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.4794817416351</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55.69584491876034</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2112915592"/>
+        <c:axId val="2114501400"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2112915592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Password</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Method</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2114501400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2114501400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Log_10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Average Entropy</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2112915592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Results by Trial</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0785439632545932"/>
+          <c:y val="0.0462962962962963"/>
+          <c:w val="0.709607174103237"/>
+          <c:h val="0.822469378827647"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>RS</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Avg Tests'!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>First Trial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Second Trial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Avg Tests'!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.455625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.713125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>MPM</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Avg Tests'!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>First Trial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Second Trial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Avg Tests'!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>MX</c:v>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Avg Tests'!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>First Trial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Second Trial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Avg Tests'!$D$2:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.805625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2117273400"/>
+        <c:axId val="2117766248"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2117273400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2117766248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2117766248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>SImilarity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2117273400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Learning</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Gains</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Learning Gains'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Improvement</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Learning Gains'!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>RS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MX</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Learning Gains'!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.294285714285714</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.518333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2110858536"/>
+        <c:axId val="2114775832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2110858536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2114775832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2114775832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Percent Change Similarity</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2110858536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1207,10 +2047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1358,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <f>STDEV(E2,G2)</f>
+        <f t="shared" ref="J2:J9" si="0">STDEV(E2,G2)</f>
         <v>0</v>
       </c>
       <c r="K2" t="s">
@@ -1431,7 +2271,7 @@
         <v>25</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="0">94^10</f>
+        <f t="shared" ref="C3:C9" si="1">94^10</f>
         <v>5.3861511409489969E+19</v>
       </c>
       <c r="D3" t="s">
@@ -1449,15 +2289,15 @@
         <v>0.86</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H9" si="1">G3-E3</f>
+        <f t="shared" ref="H3:H9" si="2">G3-E3</f>
         <v>0.39500000000000002</v>
       </c>
       <c r="I3">
-        <f>(E3+G3)/2</f>
+        <f t="shared" ref="I3:I9" si="3">(E3+G3)/2</f>
         <v>0.66249999999999998</v>
       </c>
       <c r="J3">
-        <f>STDEV(E3,G3)</f>
+        <f t="shared" si="0"/>
         <v>0.27930717856868614</v>
       </c>
       <c r="K3" t="s">
@@ -1486,14 +2326,14 @@
         <v>1</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S9" si="2">STDEV(N3,P3)</f>
+        <f t="shared" ref="S3:S9" si="4">STDEV(N3,P3)</f>
         <v>0</v>
       </c>
       <c r="T3" t="s">
         <v>29</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U9" si="3">26^LEN(T3)</f>
+        <f t="shared" ref="U3:U9" si="5">26^LEN(T3)</f>
         <v>1.9017224572684885E+45</v>
       </c>
       <c r="V3" t="s">
@@ -1518,7 +2358,7 @@
         <v>0.79249999999999998</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB9" si="4">STDEV(W3, Y3)</f>
+        <f t="shared" ref="AB3:AB9" si="6">STDEV(W3, Y3)</f>
         <v>0.29344931419241727</v>
       </c>
       <c r="AC3" t="s">
@@ -1533,7 +2373,7 @@
         <v>32</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3861511409489969E+19</v>
       </c>
       <c r="D4" t="s">
@@ -1550,15 +2390,15 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.52500000000000002</v>
       </c>
       <c r="I4">
-        <f>(E4+G4)/2</f>
+        <f t="shared" si="3"/>
         <v>0.73750000000000004</v>
       </c>
       <c r="J4">
-        <f>STDEV(E4,G4)</f>
+        <f t="shared" si="0"/>
         <v>0.37123106012293733</v>
       </c>
       <c r="K4" t="s">
@@ -1587,14 +2427,14 @@
         <v>1</v>
       </c>
       <c r="S4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T4" t="s">
         <v>27</v>
       </c>
       <c r="U4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.6005910908538611E+38</v>
       </c>
       <c r="V4" t="s">
@@ -1616,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC4" t="s">
@@ -1631,7 +2471,7 @@
         <v>42</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3861511409489969E+19</v>
       </c>
       <c r="D5" t="s">
@@ -1649,15 +2489,15 @@
         <v>0.57000000000000006</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.29500000000000004</v>
       </c>
       <c r="I5">
-        <f>(E5+G5)/2</f>
+        <f t="shared" si="3"/>
         <v>0.42250000000000004</v>
       </c>
       <c r="J5">
-        <f>STDEV(E5,G5)</f>
+        <f t="shared" si="0"/>
         <v>0.20859650045003153</v>
       </c>
       <c r="K5" t="s">
@@ -1686,14 +2526,14 @@
         <v>1</v>
       </c>
       <c r="S5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T5" t="s">
         <v>39</v>
       </c>
       <c r="U5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.1561195802071578E+36</v>
       </c>
       <c r="V5" t="s">
@@ -1715,7 +2555,7 @@
         <v>1</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC5" t="s">
@@ -1730,7 +2570,7 @@
         <v>40</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3861511409489969E+19</v>
       </c>
       <c r="D6" t="s">
@@ -1748,15 +2588,15 @@
         <v>0.7</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="I6">
-        <f>(E6+G6)/2</f>
+        <f t="shared" si="3"/>
         <v>0.69</v>
       </c>
       <c r="J6">
-        <f>STDEV(E6,G6)</f>
+        <f t="shared" si="0"/>
         <v>1.4142135623730963E-2</v>
       </c>
       <c r="K6" t="s">
@@ -1785,14 +2625,14 @@
         <v>1</v>
       </c>
       <c r="S6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T6" t="s">
         <v>38</v>
       </c>
       <c r="U6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.6904152163272471E+50</v>
       </c>
       <c r="V6" t="s">
@@ -1814,7 +2654,7 @@
         <v>1</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC6" t="s">
@@ -1829,7 +2669,7 @@
         <v>48</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3861511409489969E+19</v>
       </c>
       <c r="D7" t="s">
@@ -1847,15 +2687,15 @@
         <v>0.15</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="I7">
-        <f>(E7+G7)/2</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="J7">
-        <f>STDEV(E7,G7)</f>
+        <f t="shared" si="0"/>
         <v>7.0710678118654738E-2</v>
       </c>
       <c r="K7" t="s">
@@ -1884,14 +2724,14 @@
         <v>1</v>
       </c>
       <c r="S7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>52</v>
       </c>
       <c r="U7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.1561195802071578E+36</v>
       </c>
       <c r="V7" t="s">
@@ -1916,7 +2756,7 @@
         <v>0.78249999999999997</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.30759144981614817</v>
       </c>
       <c r="AC7" t="s">
@@ -1931,7 +2771,7 @@
         <v>57</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3861511409489969E+19</v>
       </c>
       <c r="D8" t="s">
@@ -1949,15 +2789,15 @@
         <v>0.67500000000000004</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.45000000000000007</v>
       </c>
       <c r="I8">
-        <f>(E8+G8)/2</f>
+        <f t="shared" si="3"/>
         <v>0.45</v>
       </c>
       <c r="J8">
-        <f>STDEV(E8,G8)</f>
+        <f t="shared" si="0"/>
         <v>0.31819805153394648</v>
       </c>
       <c r="K8" t="s">
@@ -1986,14 +2826,14 @@
         <v>1</v>
       </c>
       <c r="S8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T8" t="s">
         <v>53</v>
       </c>
       <c r="U8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.3424673908950952E+49</v>
       </c>
       <c r="V8" t="s">
@@ -2015,7 +2855,7 @@
         <v>1</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC8" t="s">
@@ -2030,7 +2870,7 @@
         <v>63</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3861511409489969E+19</v>
       </c>
       <c r="D9" t="s">
@@ -2048,15 +2888,15 @@
         <v>0.75</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.27500000000000002</v>
       </c>
       <c r="I9">
-        <f>(E9+G9)/2</f>
+        <f t="shared" si="3"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="J9">
-        <f>STDEV(E9,G9)</f>
+        <f t="shared" si="0"/>
         <v>0.19445436482630007</v>
       </c>
       <c r="K9" t="s">
@@ -2085,14 +2925,14 @@
         <v>1</v>
       </c>
       <c r="S9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T9" s="2" t="s">
         <v>61</v>
       </c>
       <c r="U9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.9713111838963607E+56</v>
       </c>
       <c r="V9" t="s">
@@ -2117,7 +2957,7 @@
         <v>0.64749999999999996</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.49851028073651604</v>
       </c>
       <c r="AC9" t="s">
@@ -2141,8 +2981,8 @@
         <v>0.71312500000000001</v>
       </c>
       <c r="H10">
-        <f>AVERAGE(H2:H9)</f>
-        <v>0.25750000000000001</v>
+        <f>AVERAGE(H3:H9)</f>
+        <v>0.29428571428571432</v>
       </c>
       <c r="I10">
         <f>AVERAGE(I2:I9)</f>
@@ -2198,6 +3038,16 @@
       <c r="AB10">
         <f>AVERAGE(AB2:AB9)</f>
         <v>0.13744388059313517</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="E11">
+        <f>STDEV(E2:E9)</f>
+        <v>0.29225035133792893</v>
+      </c>
+      <c r="G11">
+        <f>STDEV(G2:G9)</f>
+        <v>0.27431652077741969</v>
       </c>
     </row>
   </sheetData>
@@ -2209,4 +3059,192 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2">
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="C2">
+        <f>LOG10(B2)</f>
+        <v>19.731278535996985</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3">
+        <v>3016350058800</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C4" si="0">LOG10(B3)</f>
+        <v>12.479481741635102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4">
+        <v>4.9641502607216668E+55</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>55.695844918760336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2">
+        <v>0.45562499999999995</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.80562500000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3">
+        <v>0.71312500000000001</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2">
+        <v>0.29428571428571432</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3">
+        <v>0.51833333333333342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Started running tests with Hashcat to break md5 hashes. makehashes.py script was used to make the hashes, results of time it takes to break the hashes stored in results.xlsx
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1460" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Entropy Graph" sheetId="2" r:id="rId2"/>
     <sheet name="Avg Tests" sheetId="3" r:id="rId3"/>
     <sheet name="Learning Gains" sheetId="4" r:id="rId4"/>
+    <sheet name="Password Cracking" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -84,18 +85,6 @@
     <t>Exp Order</t>
   </si>
   <si>
-    <t>MPM, MX, RS</t>
-  </si>
-  <si>
-    <t>alotbsol85</t>
-  </si>
-  <si>
-    <t>evildolphinbitesuglyshoe</t>
-  </si>
-  <si>
-    <t>JUs9l^@6t$</t>
-  </si>
-  <si>
     <t>RS, MX, MPM</t>
   </si>
   <si>
@@ -286,6 +275,51 @@
   </si>
   <si>
     <t>Improvement</t>
+  </si>
+  <si>
+    <t>Attack Mask</t>
+  </si>
+  <si>
+    <t>?l?l?l?l?d?d?d?d</t>
+  </si>
+  <si>
+    <t>Passes cracked</t>
+  </si>
+  <si>
+    <t>?l?l?l?l?d?d</t>
+  </si>
+  <si>
+    <t>MS-3,MS-5</t>
+  </si>
+  <si>
+    <t>Attacking with pw-min set to the right number mask attack</t>
+  </si>
+  <si>
+    <t>User Time (hh:mm:ss)</t>
+  </si>
+  <si>
+    <t>MS-1,MS-2</t>
+  </si>
+  <si>
+    <t>?a*10</t>
+  </si>
+  <si>
+    <t>&gt; 10 years (predicted)</t>
+  </si>
+  <si>
+    <t>?l?l?l?l?l?d?d</t>
+  </si>
+  <si>
+    <t>?l?l?l?l?l?l?d?d?d?d</t>
+  </si>
+  <si>
+    <t>approx 5 days (pred.)</t>
+  </si>
+  <si>
+    <t>2:41.21</t>
+  </si>
+  <si>
+    <t>MS-6, MS-7</t>
   </si>
 </sst>
 </file>
@@ -354,7 +388,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="311">
+  <cellStyleXfs count="319">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -666,16 +700,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="311">
+  <cellStyles count="319">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -831,6 +875,10 @@
     <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -986,6 +1034,10 @@
     <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1098,11 +1150,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2112915592"/>
-        <c:axId val="2114501400"/>
+        <c:axId val="2086503368"/>
+        <c:axId val="2086515368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2112915592"/>
+        <c:axId val="2086503368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,7 +1187,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114501400"/>
+        <c:crossAx val="2086515368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1143,7 +1195,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2114501400"/>
+        <c:axId val="2086515368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1177,7 +1229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112915592"/>
+        <c:crossAx val="2086503368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1369,11 +1421,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117273400"/>
-        <c:axId val="2117766248"/>
+        <c:axId val="2086594680"/>
+        <c:axId val="2086597656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117273400"/>
+        <c:axId val="2086594680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1382,7 +1434,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117766248"/>
+        <c:crossAx val="2086597656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1390,7 +1442,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117766248"/>
+        <c:axId val="2086597656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1427,7 +1479,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117273400"/>
+        <c:crossAx val="2086594680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1548,11 +1600,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2110858536"/>
-        <c:axId val="2114775832"/>
+        <c:axId val="2086634232"/>
+        <c:axId val="2086637176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110858536"/>
+        <c:axId val="2086634232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,7 +1613,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114775832"/>
+        <c:crossAx val="2086637176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1569,7 +1621,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2114775832"/>
+        <c:axId val="2086637176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1603,7 +1655,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110858536"/>
+        <c:crossAx val="2086634232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2047,10 +2099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC11"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2086,7 +2138,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2101,19 +2153,19 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>6</v>
@@ -2128,19 +2180,19 @@
         <v>9</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>14</v>
@@ -2155,13 +2207,13 @@
         <v>17</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>19</v>
@@ -2169,95 +2221,101 @@
     </row>
     <row r="2" spans="1:29">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C8" si="0">94^10</f>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <f>(0.43 + 0.5) / 2</f>
+        <v>0.46499999999999997</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2">
+        <f>(0.9 + 0.82)/2</f>
+        <v>0.86</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:H8" si="1">G2-E2</f>
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I8" si="2">(E2+G2)/2</f>
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J8" si="3">STDEV(E2,G2)</f>
+        <v>0.27930717856868614</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2">
+        <f>(26^4)*(10^4)</f>
+        <v>4569760000</v>
+      </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <f t="shared" ref="S2:S8" si="4">STDEV(N2,P2)</f>
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2">
-        <f>94^10</f>
-        <v>5.3861511409489969E+19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <f>G2-E2</f>
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <f t="shared" ref="J2:J9" si="0">STDEV(E2,G2)</f>
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2">
-        <f>(26^8)*(10^2)</f>
-        <v>20882706457600</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>75</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <f>STDEV(N2,P2)</f>
-        <v>0</v>
-      </c>
       <c r="T2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="U2">
-        <f>26^LEN(T2)</f>
-        <v>9.1066857695372161E+33</v>
+        <f t="shared" ref="U2:U8" si="5">26^LEN(T2)</f>
+        <v>1.9017224572684885E+45</v>
       </c>
       <c r="V2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <f>(0.42 + 0.75)/2</f>
+        <v>0.58499999999999996</v>
       </c>
       <c r="X2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="Y2">
         <v>1</v>
       </c>
-      <c r="Z2" t="s">
-        <v>75</v>
+      <c r="Z2">
+        <f>Y2-W2</f>
+        <v>0.41500000000000004</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <f>(W2+Y2)/2</f>
+        <v>0.79249999999999998</v>
       </c>
       <c r="AB2">
-        <f>STDEV(W2, Y2)</f>
-        <v>0</v>
+        <f t="shared" ref="AB2:AB8" si="6">STDEV(W2, Y2)</f>
+        <v>0.29344931419241727</v>
       </c>
       <c r="AC2" t="s">
         <v>20</v>
@@ -2265,163 +2323,160 @@
     </row>
     <row r="3" spans="1:29">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C9" si="1">94^10</f>
+        <f t="shared" si="0"/>
         <v>5.3861511409489969E+19</v>
       </c>
       <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <f>(0.45+0.5)/2</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="E3">
-        <f>(0.43 + 0.5) / 2</f>
-        <v>0.46499999999999997</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="2"/>
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="3"/>
+        <v>0.37123106012293733</v>
+      </c>
+      <c r="K3" t="s">
         <v>30</v>
-      </c>
-      <c r="G3">
-        <f>(0.9 + 0.82)/2</f>
-        <v>0.86</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H9" si="2">G3-E3</f>
-        <v>0.39500000000000002</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I9" si="3">(E3+G3)/2</f>
-        <v>0.66249999999999998</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
-        <v>0.27930717856868614</v>
-      </c>
-      <c r="K3" t="s">
-        <v>35</v>
       </c>
       <c r="L3">
         <f>(26^4)*(10^4)</f>
         <v>4569760000</v>
       </c>
       <c r="M3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="P3">
         <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S9" si="4">STDEV(N3,P3)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U9" si="5">26^LEN(T3)</f>
-        <v>1.9017224572684885E+45</v>
+        <f t="shared" si="5"/>
+        <v>1.6005910908538611E+38</v>
       </c>
       <c r="V3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="W3">
-        <f>(0.42 + 0.75)/2</f>
-        <v>0.58499999999999996</v>
+        <v>1</v>
       </c>
       <c r="X3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Y3">
         <v>1</v>
       </c>
-      <c r="Z3">
-        <f>Y3-W3</f>
-        <v>0.41500000000000004</v>
+      <c r="Z3" t="s">
+        <v>71</v>
       </c>
       <c r="AA3">
-        <f>(W3+Y3)/2</f>
-        <v>0.79249999999999998</v>
+        <v>1</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB9" si="6">STDEV(W3, Y3)</f>
-        <v>0.29344931419241727</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="AC3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C4">
+        <f t="shared" si="0"/>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <f>(0.25 + 0.3)/2</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4">
+        <f>(0.6+0.54)/2</f>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="1"/>
-        <v>5.3861511409489969E+19</v>
-      </c>
-      <c r="D4" t="s">
+        <v>0.29500000000000004</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0.42250000000000004</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>0.20859650045003153</v>
+      </c>
+      <c r="K4" t="s">
         <v>33</v>
       </c>
-      <c r="E4">
-        <f>(0.45+0.5)/2</f>
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="2"/>
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="3"/>
-        <v>0.73750000000000004</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>0.37123106012293733</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
       <c r="L4">
-        <f>(26^4)*(10^4)</f>
-        <v>4569760000</v>
+        <f>(26^4)*(10^2)</f>
+        <v>45697600</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P4">
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="R4">
         <v>1</v>
@@ -2431,26 +2486,26 @@
         <v>0</v>
       </c>
       <c r="T4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="U4">
         <f t="shared" si="5"/>
-        <v>1.6005910908538611E+38</v>
+        <v>6.1561195802071578E+36</v>
       </c>
       <c r="V4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="W4">
         <v>1</v>
       </c>
       <c r="X4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="Y4">
         <v>1</v>
       </c>
       <c r="Z4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="AA4">
         <v>1</v>
@@ -2460,67 +2515,67 @@
         <v>0</v>
       </c>
       <c r="AC4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C5">
+        <f t="shared" si="0"/>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <f>(0.95 + 0.41)/2</f>
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5">
+        <f>(0.95 + 0.45)/2</f>
+        <v>0.7</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="1"/>
-        <v>5.3861511409489969E+19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5">
-        <f>(0.25 + 0.3)/2</f>
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5">
-        <f>(0.6+0.54)/2</f>
-        <v>0.57000000000000006</v>
-      </c>
-      <c r="H5">
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="I5">
         <f t="shared" si="2"/>
-        <v>0.29500000000000004</v>
-      </c>
-      <c r="I5">
+        <v>0.69</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="3"/>
-        <v>0.42250000000000004</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>0.20859650045003153</v>
+        <v>1.4142135623730963E-2</v>
       </c>
       <c r="K5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L5">
-        <f>(26^4)*(10^2)</f>
-        <v>45697600</v>
+        <f>(26^6)*(10^4)</f>
+        <v>3089157760000</v>
       </c>
       <c r="M5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="N5">
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="P5">
         <v>1</v>
       </c>
       <c r="Q5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="R5">
         <v>1</v>
@@ -2530,26 +2585,26 @@
         <v>0</v>
       </c>
       <c r="T5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="U5">
         <f t="shared" si="5"/>
-        <v>6.1561195802071578E+36</v>
+        <v>8.6904152163272471E+50</v>
       </c>
       <c r="V5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="W5">
         <v>1</v>
       </c>
       <c r="X5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="Y5">
         <v>1</v>
       </c>
       <c r="Z5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="AA5">
         <v>1</v>
@@ -2559,67 +2614,67 @@
         <v>0</v>
       </c>
       <c r="AC5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
       </c>
       <c r="C6">
+        <f t="shared" si="0"/>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <f>0.1/2</f>
+        <v>0.05</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6">
+        <f>0.3/2</f>
+        <v>0.15</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="1"/>
-        <v>5.3861511409489969E+19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6">
-        <f>(0.95 + 0.41)/2</f>
-        <v>0.67999999999999994</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6">
-        <f>(0.95 + 0.45)/2</f>
-        <v>0.7</v>
-      </c>
-      <c r="H6">
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="2"/>
-        <v>2.0000000000000018E-2</v>
-      </c>
-      <c r="I6">
+        <v>0.1</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="3"/>
-        <v>0.69</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1.4142135623730963E-2</v>
+        <v>7.0710678118654738E-2</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L6">
-        <f>(26^6)*(10^4)</f>
-        <v>3089157760000</v>
+        <f>(26^4)*(10^2)</f>
+        <v>45697600</v>
       </c>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P6">
         <v>1</v>
       </c>
       <c r="Q6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="R6">
         <v>1</v>
@@ -2628,97 +2683,100 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T6" t="s">
-        <v>38</v>
+      <c r="T6" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="U6">
         <f t="shared" si="5"/>
-        <v>8.6904152163272471E+50</v>
+        <v>6.1561195802071578E+36</v>
       </c>
       <c r="V6" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="W6">
-        <v>1</v>
-      </c>
-      <c r="X6" t="s">
-        <v>38</v>
+        <f>(0.38 + 0.75)/2</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="Y6">
         <v>1</v>
       </c>
-      <c r="Z6" t="s">
-        <v>75</v>
+      <c r="Z6">
+        <f>Y6-W6</f>
+        <v>0.43500000000000005</v>
       </c>
       <c r="AA6">
-        <v>1</v>
+        <f>(W6+Y6)/2</f>
+        <v>0.78249999999999997</v>
       </c>
       <c r="AB6">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.30759144981614817</v>
       </c>
       <c r="AC6" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C7">
+        <f t="shared" si="0"/>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7">
+        <f>0.45/2</f>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7">
+        <f>(0.9+0.45)/2</f>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="1"/>
-        <v>5.3861511409489969E+19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7">
-        <f>0.1/2</f>
-        <v>0.05</v>
-      </c>
-      <c r="F7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7">
-        <f>0.3/2</f>
-        <v>0.15</v>
-      </c>
-      <c r="H7">
+        <v>0.45000000000000007</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="2"/>
-        <v>9.9999999999999992E-2</v>
-      </c>
-      <c r="I7">
+        <v>0.45</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>7.0710678118654738E-2</v>
+        <v>0.31819805153394648</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L7">
-        <f>(26^4)*(10^2)</f>
-        <v>45697600</v>
+        <f>(26^6)*(10^2)</f>
+        <v>30891577600</v>
       </c>
       <c r="M7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N7">
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P7">
         <v>1</v>
       </c>
       <c r="Q7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="R7">
         <v>1</v>
@@ -2727,85 +2785,82 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T7" s="3" t="s">
-        <v>52</v>
+      <c r="T7" t="s">
+        <v>49</v>
       </c>
       <c r="U7">
         <f t="shared" si="5"/>
-        <v>6.1561195802071578E+36</v>
+        <v>3.3424673908950952E+49</v>
       </c>
       <c r="V7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="W7">
-        <f>(0.38 + 0.75)/2</f>
-        <v>0.56499999999999995</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>52</v>
+        <v>1</v>
+      </c>
+      <c r="X7" t="s">
+        <v>49</v>
       </c>
       <c r="Y7">
         <v>1</v>
       </c>
-      <c r="Z7">
-        <f>Y7-W7</f>
-        <v>0.43500000000000005</v>
+      <c r="Z7" t="s">
+        <v>71</v>
       </c>
       <c r="AA7">
-        <f>(W7+Y7)/2</f>
-        <v>0.78249999999999997</v>
+        <v>1</v>
       </c>
       <c r="AB7">
         <f t="shared" si="6"/>
-        <v>0.30759144981614817</v>
+        <v>0</v>
       </c>
       <c r="AC7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C8">
+        <f t="shared" si="0"/>
+        <v>5.3861511409489969E+19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8">
+        <f>(0.6 + 0.35)/2</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8">
+        <f>(0.7+0.8)/2</f>
+        <v>0.75</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="1"/>
-        <v>5.3861511409489969E+19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8">
-        <f>0.45/2</f>
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="F8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8">
-        <f>(0.9+0.45)/2</f>
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="H8">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="2"/>
-        <v>0.45000000000000007</v>
-      </c>
-      <c r="I8">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="3"/>
-        <v>0.45</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>0.31819805153394648</v>
+        <v>0.19445436482630007</v>
       </c>
       <c r="K8" t="s">
         <v>56</v>
       </c>
       <c r="L8">
-        <f>(26^6)*(10^2)</f>
-        <v>30891577600</v>
+        <f>(26^5)*(10^4)</f>
+        <v>118813760000</v>
       </c>
       <c r="M8" t="s">
         <v>56</v>
@@ -2820,7 +2875,7 @@
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="R8">
         <v>1</v>
@@ -2829,225 +2884,126 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T8" t="s">
-        <v>53</v>
+      <c r="T8" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="U8">
         <f t="shared" si="5"/>
-        <v>3.3424673908950952E+49</v>
+        <v>3.9713111838963607E+56</v>
       </c>
       <c r="V8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="W8">
-        <v>1</v>
-      </c>
-      <c r="X8" t="s">
-        <v>53</v>
+        <f>(0.5 + 0.09)/2</f>
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="Y8">
         <v>1</v>
       </c>
-      <c r="Z8" t="s">
-        <v>75</v>
+      <c r="Z8">
+        <f>Y8-W8</f>
+        <v>0.70500000000000007</v>
       </c>
       <c r="AA8">
-        <v>1</v>
+        <f>(W8+Y8)/2</f>
+        <v>0.64749999999999996</v>
       </c>
       <c r="AB8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.49851028073651604</v>
       </c>
       <c r="AC8" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:29">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
+      <c r="A9" t="s">
+        <v>64</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
-        <v>5.3861511409489969E+19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>64</v>
+        <f>AVERAGE(C2:C8)</f>
+        <v>5.3861511409489977E+19</v>
       </c>
       <c r="E9">
-        <f>(0.6 + 0.35)/2</f>
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="F9" t="s">
-        <v>65</v>
+        <f>AVERAGE(E2:E8)</f>
+        <v>0.37785714285714284</v>
       </c>
       <c r="G9">
-        <f>(0.7+0.8)/2</f>
-        <v>0.75</v>
+        <f>AVERAGE(G2:G8)</f>
+        <v>0.67214285714285715</v>
       </c>
       <c r="H9">
-        <f t="shared" si="2"/>
-        <v>0.27500000000000002</v>
+        <f>AVERAGE(H2:H8)</f>
+        <v>0.29428571428571432</v>
       </c>
       <c r="I9">
-        <f t="shared" si="3"/>
-        <v>0.61250000000000004</v>
+        <f>AVERAGE(I2:I8)</f>
+        <v>0.52500000000000013</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
-        <v>0.19445436482630007</v>
-      </c>
-      <c r="K9" t="s">
-        <v>60</v>
+        <f>AVERAGE(J2:J8)</f>
+        <v>0.20809142417775531</v>
       </c>
       <c r="L9">
-        <f>(26^5)*(10^4)</f>
-        <v>118813760000</v>
-      </c>
-      <c r="M9" t="s">
-        <v>60</v>
+        <f>AVERAGE(L2:L8)</f>
+        <v>464013430400</v>
       </c>
       <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9" t="s">
-        <v>60</v>
+        <f>AVERAGE(N2:N8)</f>
+        <v>1</v>
       </c>
       <c r="P9">
+        <f>AVERAGE(P2:P8)</f>
         <v>1</v>
       </c>
       <c r="Q9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="R9">
+        <f>AVERAGE(R2:R8)</f>
         <v>1</v>
       </c>
       <c r="S9">
-        <f t="shared" si="4"/>
+        <f>AVERAGE(S2:S8)</f>
         <v>0</v>
       </c>
-      <c r="T9" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="U9">
-        <f t="shared" si="5"/>
-        <v>3.9713111838963607E+56</v>
-      </c>
-      <c r="V9" t="s">
-        <v>62</v>
+        <f>AVERAGE(U2:U8)</f>
+        <v>5.673314583681905E+55</v>
       </c>
       <c r="W9">
-        <f>(0.5 + 0.09)/2</f>
-        <v>0.29499999999999998</v>
-      </c>
-      <c r="X9" s="2" t="s">
-        <v>61</v>
+        <f>AVERAGE(W2:W8)</f>
+        <v>0.77785714285714291</v>
       </c>
       <c r="Y9">
+        <f>AVERAGE(Y2:Y8)</f>
         <v>1</v>
       </c>
       <c r="Z9">
-        <f>Y9-W9</f>
-        <v>0.70500000000000007</v>
+        <f>AVERAGE(Z2,Z6,Z8)</f>
+        <v>0.51833333333333342</v>
       </c>
       <c r="AA9">
-        <f>(W9+Y9)/2</f>
-        <v>0.64749999999999996</v>
+        <f>AVERAGE(AA2:AA8)</f>
+        <v>0.8889285714285714</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="6"/>
-        <v>0.49851028073651604</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>36</v>
+        <f>AVERAGE(AB2:AB8)</f>
+        <v>0.15707872067786877</v>
       </c>
     </row>
     <row r="10" spans="1:29">
-      <c r="A10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10">
-        <f>AVERAGE(C2:C9)</f>
-        <v>5.3861511409489969E+19</v>
-      </c>
       <c r="E10">
-        <f>AVERAGE(E2:E9)</f>
-        <v>0.45562499999999995</v>
+        <f>STDEV(E2:E8)</f>
+        <v>0.20784323304791402</v>
       </c>
       <c r="G10">
-        <f>AVERAGE(G2:G9)</f>
-        <v>0.71312500000000001</v>
-      </c>
-      <c r="H10">
-        <f>AVERAGE(H3:H9)</f>
-        <v>0.29428571428571432</v>
-      </c>
-      <c r="I10">
-        <f>AVERAGE(I2:I9)</f>
-        <v>0.58437499999999998</v>
-      </c>
-      <c r="J10">
-        <f>AVERAGE(J2:J9)</f>
-        <v>0.18207999615553588</v>
-      </c>
-      <c r="L10">
-        <f>AVERAGE(L2:L9)</f>
-        <v>3016350058800</v>
-      </c>
-      <c r="N10">
-        <f>AVERAGE(N2:N9)</f>
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <f>AVERAGE(P2:P9)</f>
-        <v>1</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>75</v>
-      </c>
-      <c r="R10">
-        <f>AVERAGE(R2:R9)</f>
-        <v>1</v>
-      </c>
-      <c r="S10">
-        <f>AVERAGE(S2:S9)</f>
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <f>AVERAGE(U2:U9)</f>
-        <v>4.9641502607216668E+55</v>
-      </c>
-      <c r="W10">
-        <f>AVERAGE(W2:W9)</f>
-        <v>0.80562500000000004</v>
-      </c>
-      <c r="Y10">
-        <f>AVERAGE(Y2:Y9)</f>
-        <v>1</v>
-      </c>
-      <c r="Z10">
-        <f>AVERAGE(Z3,Z7,Z9)</f>
-        <v>0.51833333333333342</v>
-      </c>
-      <c r="AA10">
-        <f>AVERAGE(AA2:AA9)</f>
-        <v>0.90281250000000002</v>
-      </c>
-      <c r="AB10">
-        <f>AVERAGE(AB2:AB9)</f>
-        <v>0.13744388059313517</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29">
-      <c r="E11">
-        <f>STDEV(E2:E9)</f>
-        <v>0.29225035133792893</v>
-      </c>
-      <c r="G11">
-        <f>STDEV(G2:G9)</f>
-        <v>0.27431652077741969</v>
+        <f>STDEV(G2:G8)</f>
+        <v>0.26854324826827447</v>
       </c>
     </row>
   </sheetData>
@@ -3078,18 +3034,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <v>5.3861511409489969E+19</v>
@@ -3101,7 +3057,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B3">
         <v>3016350058800</v>
@@ -3113,7 +3069,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B4">
         <v>4.9641502607216668E+55</v>
@@ -3149,21 +3105,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B2">
         <v>0.45562499999999995</v>
@@ -3177,7 +3133,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B3">
         <v>0.71312500000000001</v>
@@ -3205,8 +3161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3216,15 +3172,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <v>0.29428571428571432</v>
@@ -3232,7 +3188,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B3">
         <v>0.51833333333333342</v>
@@ -3247,4 +3203,95 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2">
+        <v>5.88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.3979166666666667</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="G12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
First figure and table
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1460" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -388,8 +388,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="319">
+  <cellStyleXfs count="323">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -719,7 +723,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="319">
+  <cellStyles count="323">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -879,6 +883,8 @@
     <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1038,6 +1044,8 @@
     <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1070,7 +1078,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Entropy</a:t>
+              <a:t>Log Entropy</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -1132,10 +1140,10 @@
                   <c:v>19.73127853599699</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.4794817416351</c:v>
+                  <c:v>11.66653055095186</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.69584491876034</c:v>
+                  <c:v>55.75383686573802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1150,11 +1158,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2086503368"/>
-        <c:axId val="2086515368"/>
+        <c:axId val="2111578952"/>
+        <c:axId val="2111589144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2086503368"/>
+        <c:axId val="2111578952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1167,17 +1175,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1600"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>Password</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> Method</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1187,7 +1195,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086515368"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2111589144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1195,7 +1213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086515368"/>
+        <c:axId val="2111589144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1208,17 +1226,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>Log_10</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> Average Entropy</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1229,7 +1247,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086503368"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2111578952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1281,7 +1309,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1421,11 +1448,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2086594680"/>
-        <c:axId val="2086597656"/>
+        <c:axId val="2106296728"/>
+        <c:axId val="2106299704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2086594680"/>
+        <c:axId val="2106296728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1434,7 +1461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086597656"/>
+        <c:crossAx val="2106299704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1442,7 +1469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086597656"/>
+        <c:axId val="2106299704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1472,21 +1499,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086594680"/>
+        <c:crossAx val="2106296728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1536,7 +1561,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1600,11 +1624,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2086634232"/>
-        <c:axId val="2086637176"/>
+        <c:axId val="2105570024"/>
+        <c:axId val="2105572968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2086634232"/>
+        <c:axId val="2105570024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,7 +1637,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086637176"/>
+        <c:crossAx val="2105572968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1621,7 +1645,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086637176"/>
+        <c:axId val="2105572968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1648,14 +1672,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086634232"/>
+        <c:crossAx val="2105570024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1676,16 +1699,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2101,8 +2124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3019,10 +3042,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3030,9 +3053,11 @@
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -3043,7 +3068,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -3054,29 +3079,85 @@
         <f>LOG10(B2)</f>
         <v>19.731278535996985</v>
       </c>
+      <c r="J2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>75</v>
       </c>
       <c r="B3">
-        <v>3016350058800</v>
+        <v>464013430400</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C4" si="0">LOG10(B3)</f>
-        <v>12.479481741635102</v>
+        <v>11.666530550951858</v>
+      </c>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3">
+        <f>B2/B2</f>
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f>B3/B2</f>
+        <v>8.6149351969028577E-9</v>
+      </c>
+      <c r="L3">
+        <f>B4/B2</f>
+        <v>1.0533151475363745E+36</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>76</v>
       </c>
       <c r="B4">
-        <v>4.9641502607216668E+55</v>
+        <v>5.673314583681905E+55</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>55.695844918760336</v>
+        <v>55.753836865738023</v>
+      </c>
+      <c r="I4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4">
+        <f>B2/B3</f>
+        <v>116077483.71218258</v>
+      </c>
+      <c r="K4">
+        <f>B3/B3</f>
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <f>B4/B3</f>
+        <v>1.2226617188194872E+44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="I5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5">
+        <f>B2/B4</f>
+        <v>9.4938347971063104E-37</v>
+      </c>
+      <c r="K5">
+        <f>B3/B4</f>
+        <v>8.1788771547172259E-45</v>
+      </c>
+      <c r="L5">
+        <f>B4/B4</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Second figure and grahp
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1460" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="323">
+  <cellStyleXfs count="329">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -712,8 +712,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -722,8 +728,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="323">
+  <cellStyles count="329">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -885,6 +892,9 @@
     <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1046,6 +1056,9 @@
     <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1309,6 +1322,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1318,8 +1332,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0785439632545932"/>
-          <c:y val="0.0462962962962963"/>
+          <c:x val="0.127416079569001"/>
+          <c:y val="0.0436716473432947"/>
           <c:w val="0.709607174103237"/>
           <c:h val="0.822469378827647"/>
         </c:manualLayout>
@@ -1354,10 +1368,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.455625</c:v>
+                  <c:v>0.377857142857143</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.713125</c:v>
+                  <c:v>0.672142857142857</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1428,7 +1442,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.805625</c:v>
+                  <c:v>0.777857142857143</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
@@ -1461,6 +1475,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="2106299704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -1485,26 +1509,44 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>Average</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>SImilarity</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0169165531940086"/>
+              <c:y val="0.305299977266621"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="2106296728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -1512,7 +1554,18 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1734,14 +1787,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
@@ -2124,8 +2177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3044,8 +3097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3130,7 +3183,7 @@
       <c r="I4" t="s">
         <v>75</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="6">
         <f>B2/B3</f>
         <v>116077483.71218258</v>
       </c>
@@ -3175,8 +3228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3203,13 +3256,13 @@
         <v>81</v>
       </c>
       <c r="B2">
-        <v>0.45562499999999995</v>
+        <v>0.37785714285714284</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0.80562500000000004</v>
+        <v>0.77785714285714291</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3217,7 +3270,7 @@
         <v>80</v>
       </c>
       <c r="B3">
-        <v>0.71312500000000001</v>
+        <v>0.67214285714285715</v>
       </c>
       <c r="C3">
         <v>1</v>

</xml_diff>

<commit_message>
Added learningGains graph and table describing the time Hashcat took to run
</commit_message>
<xml_diff>
--- a/finalproject/results.xlsx
+++ b/finalproject/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1460" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1614,6 +1614,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1725,6 +1726,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2177,8 +2179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3228,7 +3230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>

</xml_diff>